<commit_message>
Add author lists; resolve #17 ; resolve #12
</commit_message>
<xml_diff>
--- a/sigmaaie/modules/core/doc/roh-core.xlsx
+++ b/sigmaaie/modules/core/doc/roh-core.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="603">
   <si>
     <t>vivo</t>
   </si>
@@ -1593,6 +1593,9 @@
   </si>
   <si>
     <t>degreeCandidacy</t>
+  </si>
+  <si>
+    <t>vivo:AdviseeRole</t>
   </si>
   <si>
     <t>FacultyMentoringRelationship</t>
@@ -2293,7 +2296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M625"/>
+  <dimension ref="A1:M626"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -11262,8 +11265,8 @@
       <c r="H544" t="s" s="41">
         <v>37</v>
       </c>
-      <c r="I544" t="s" s="45">
-        <v>220</v>
+      <c r="I544" t="s" s="41">
+        <v>527</v>
       </c>
     </row>
     <row r="545">
@@ -11271,7 +11274,7 @@
         <v>0</v>
       </c>
       <c r="D545" s="41" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E545" s="41"/>
       <c r="F545" s="41"/>
@@ -11281,7 +11284,7 @@
         <v>0</v>
       </c>
       <c r="D546" s="41" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E546" s="41"/>
       <c r="F546" s="41"/>
@@ -11291,7 +11294,7 @@
         <v>0</v>
       </c>
       <c r="D547" s="41" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E547" s="41"/>
       <c r="F547" s="41"/>
@@ -11301,7 +11304,7 @@
         <v>0</v>
       </c>
       <c r="D548" s="41" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E548" s="41"/>
       <c r="F548" s="41"/>
@@ -11311,7 +11314,7 @@
         <v>4</v>
       </c>
       <c r="C549" s="19" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D549" s="19"/>
       <c r="E549" s="19"/>
@@ -11357,7 +11360,7 @@
         <v>37</v>
       </c>
       <c r="I551" t="s" s="41">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="552">
@@ -11365,7 +11368,7 @@
         <v>0</v>
       </c>
       <c r="C552" s="41" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D552" s="41"/>
       <c r="E552" s="41"/>
@@ -11374,10 +11377,10 @@
         <v>4</v>
       </c>
       <c r="H552" t="s" s="19">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="I552" t="s" s="41">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="553">
@@ -11411,7 +11414,7 @@
         <v>37</v>
       </c>
       <c r="I554" t="s" s="41">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="555">
@@ -11466,7 +11469,7 @@
         <v>0</v>
       </c>
       <c r="C559" s="41" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D559" s="41"/>
       <c r="E559" s="41"/>
@@ -11475,7 +11478,7 @@
         <v>0</v>
       </c>
       <c r="H559" t="s" s="41">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="I559" t="s" s="45">
         <v>18</v>
@@ -11501,7 +11504,7 @@
         <v>4</v>
       </c>
       <c r="H560" t="s" s="19">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I560" t="s" s="7">
         <v>20</v>
@@ -11518,7 +11521,7 @@
         <v>4</v>
       </c>
       <c r="H561" t="s" s="20">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="I561" t="s" s="41">
         <v>15</v>
@@ -11572,7 +11575,7 @@
         <v>37</v>
       </c>
       <c r="I564" t="s" s="41">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="565">
@@ -11586,7 +11589,7 @@
         <v>0</v>
       </c>
       <c r="H565" t="s" s="41">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="I565" t="s" s="31">
         <v>115</v>
@@ -11597,7 +11600,7 @@
         <v>4</v>
       </c>
       <c r="D566" s="19" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E566" s="19"/>
       <c r="F566" s="19"/>
@@ -11607,7 +11610,7 @@
         <v>4</v>
       </c>
       <c r="D567" s="19" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E567" s="19"/>
       <c r="F567" s="19"/>
@@ -11617,7 +11620,7 @@
         <v>4</v>
       </c>
       <c r="D568" s="19" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E568" s="19"/>
       <c r="F568" s="19"/>
@@ -11627,7 +11630,7 @@
         <v>4</v>
       </c>
       <c r="D569" s="19" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E569" s="19"/>
       <c r="F569" s="19"/>
@@ -11637,7 +11640,7 @@
         <v>0</v>
       </c>
       <c r="C570" s="41" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D570" s="41"/>
       <c r="E570" s="41"/>
@@ -11655,7 +11658,7 @@
         <v>0</v>
       </c>
       <c r="K570" t="s" s="41">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="L570" t="s" s="11">
         <v>72</v>
@@ -11672,7 +11675,7 @@
         <v>4</v>
       </c>
       <c r="H571" t="s" s="20">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I571" t="s" s="45">
         <v>220</v>
@@ -11700,7 +11703,7 @@
         <v>4</v>
       </c>
       <c r="D573" s="19" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E573" s="19"/>
       <c r="F573" s="19"/>
@@ -11710,7 +11713,7 @@
         <v>4</v>
       </c>
       <c r="D574" s="19" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E574" s="19"/>
       <c r="F574" s="19"/>
@@ -11720,7 +11723,7 @@
         <v>0</v>
       </c>
       <c r="D575" s="41" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E575" s="41"/>
       <c r="F575" s="41"/>
@@ -11730,7 +11733,7 @@
         <v>0</v>
       </c>
       <c r="D576" s="41" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E576" s="41"/>
       <c r="F576" s="41"/>
@@ -11740,7 +11743,7 @@
         <v>4</v>
       </c>
       <c r="E577" s="19" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="F577" s="19"/>
     </row>
@@ -11749,7 +11752,7 @@
         <v>0</v>
       </c>
       <c r="D578" s="41" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E578" s="41"/>
       <c r="F578" s="41"/>
@@ -11759,7 +11762,7 @@
         <v>4</v>
       </c>
       <c r="E579" s="19" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F579" s="19"/>
     </row>
@@ -11768,7 +11771,7 @@
         <v>0</v>
       </c>
       <c r="D580" s="41" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E580" s="41"/>
       <c r="F580" s="41"/>
@@ -11778,7 +11781,7 @@
         <v>0</v>
       </c>
       <c r="D581" s="41" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E581" s="41"/>
       <c r="F581" s="41"/>
@@ -11788,7 +11791,7 @@
         <v>0</v>
       </c>
       <c r="E582" s="41" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F582" s="41"/>
     </row>
@@ -11797,7 +11800,7 @@
         <v>4</v>
       </c>
       <c r="D583" s="19" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E583" s="19"/>
       <c r="F583" s="19"/>
@@ -11807,7 +11810,7 @@
         <v>4</v>
       </c>
       <c r="D584" s="19" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E584" s="19"/>
       <c r="F584" s="19"/>
@@ -11817,7 +11820,7 @@
         <v>0</v>
       </c>
       <c r="D585" s="41" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E585" s="41"/>
       <c r="F585" s="41"/>
@@ -11827,7 +11830,7 @@
         <v>4</v>
       </c>
       <c r="D586" s="19" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E586" s="19"/>
       <c r="F586" s="19"/>
@@ -11837,7 +11840,7 @@
         <v>4</v>
       </c>
       <c r="D587" s="19" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E587" s="19"/>
       <c r="F587" s="19"/>
@@ -11847,7 +11850,7 @@
         <v>4</v>
       </c>
       <c r="C588" s="19" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D588" s="19"/>
       <c r="E588" s="19"/>
@@ -11893,7 +11896,7 @@
         <v>37</v>
       </c>
       <c r="I590" t="s" s="19">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="591">
@@ -11901,7 +11904,7 @@
         <v>4</v>
       </c>
       <c r="C591" s="19" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D591" s="19"/>
       <c r="E591" s="19"/>
@@ -11947,7 +11950,7 @@
         <v>37</v>
       </c>
       <c r="I593" t="s" s="41">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="594">
@@ -11955,7 +11958,7 @@
         <v>4</v>
       </c>
       <c r="D594" s="19" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E594" s="19"/>
       <c r="F594" s="19"/>
@@ -11966,7 +11969,7 @@
         <v>149</v>
       </c>
       <c r="I594" t="s" s="19">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="595">
@@ -11974,7 +11977,7 @@
         <v>4</v>
       </c>
       <c r="D595" s="19" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="E595" s="19"/>
       <c r="F595" s="19"/>
@@ -11985,7 +11988,7 @@
         <v>149</v>
       </c>
       <c r="I595" t="s" s="19">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="596">
@@ -11993,7 +11996,7 @@
         <v>4</v>
       </c>
       <c r="D596" s="19" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E596" s="19"/>
       <c r="F596" s="19"/>
@@ -12004,7 +12007,7 @@
         <v>149</v>
       </c>
       <c r="I596" t="s" s="19">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="597">
@@ -12035,7 +12038,7 @@
         <v>4</v>
       </c>
       <c r="B599" s="19" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C599" s="19"/>
       <c r="D599" s="19"/>
@@ -12047,20 +12050,20 @@
         <v>4</v>
       </c>
       <c r="B600" s="19" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C600" s="19"/>
       <c r="D600" s="19"/>
       <c r="E600" s="19"/>
       <c r="F600" s="19"/>
-      <c r="G600" t="s" s="20">
-        <v>4</v>
-      </c>
-      <c r="H600" t="s" s="20">
-        <v>324</v>
-      </c>
-      <c r="I600" t="s" s="19">
-        <v>577</v>
+      <c r="G600" t="s" s="35">
+        <v>60</v>
+      </c>
+      <c r="H600" t="s" s="35">
+        <v>297</v>
+      </c>
+      <c r="I600" t="s" s="27">
+        <v>298</v>
       </c>
     </row>
     <row r="601">
@@ -12070,117 +12073,108 @@
       <c r="D601" s="19"/>
       <c r="E601" s="19"/>
       <c r="F601" s="19"/>
-      <c r="G601" t="s" s="19">
-        <v>4</v>
-      </c>
-      <c r="H601" t="s" s="19">
-        <v>190</v>
+      <c r="G601" t="s" s="20">
+        <v>4</v>
+      </c>
+      <c r="H601" t="s" s="20">
+        <v>324</v>
       </c>
       <c r="I601" t="s" s="19">
         <v>578</v>
       </c>
     </row>
     <row r="602">
-      <c r="B602" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C602" s="19" t="s">
-        <v>579</v>
-      </c>
+      <c r="A602" s="19"/>
+      <c r="B602" s="19"/>
+      <c r="C602" s="19"/>
       <c r="D602" s="19"/>
       <c r="E602" s="19"/>
       <c r="F602" s="19"/>
+      <c r="G602" t="s" s="19">
+        <v>4</v>
+      </c>
+      <c r="H602" t="s" s="19">
+        <v>190</v>
+      </c>
+      <c r="I602" t="s" s="19">
+        <v>579</v>
+      </c>
     </row>
     <row r="603">
+      <c r="B603" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="C603" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D603" s="19" t="s">
         <v>580</v>
       </c>
+      <c r="D603" s="19"/>
       <c r="E603" s="19"/>
       <c r="F603" s="19"/>
-      <c r="J603" t="s" s="20">
-        <v>4</v>
-      </c>
-      <c r="K603" t="s" s="20">
+    </row>
+    <row r="604">
+      <c r="C604" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D604" s="19" t="s">
         <v>581</v>
       </c>
-      <c r="L603" t="s" s="11">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="604">
-      <c r="B604" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C604" s="19" t="s">
-        <v>580</v>
-      </c>
-      <c r="D604" s="19"/>
       <c r="E604" s="19"/>
       <c r="F604" s="19"/>
       <c r="J604" t="s" s="20">
         <v>4</v>
       </c>
       <c r="K604" t="s" s="20">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="L604" t="s" s="11">
         <v>515</v>
       </c>
     </row>
     <row r="605">
-      <c r="A605" s="19" t="s">
-        <v>4</v>
-      </c>
       <c r="B605" s="19" t="s">
-        <v>582</v>
-      </c>
-      <c r="C605" s="19"/>
+        <v>4</v>
+      </c>
+      <c r="C605" s="19" t="s">
+        <v>581</v>
+      </c>
       <c r="D605" s="19"/>
       <c r="E605" s="19"/>
       <c r="F605" s="19"/>
-      <c r="G605" t="s" s="41">
-        <v>0</v>
-      </c>
-      <c r="H605" t="s" s="41">
-        <v>50</v>
-      </c>
-      <c r="I605" t="s" s="41">
-        <v>51</v>
-      </c>
-      <c r="J605" t="s" s="41">
-        <v>0</v>
-      </c>
-      <c r="K605" t="s" s="41">
-        <v>13</v>
+      <c r="J605" t="s" s="20">
+        <v>4</v>
+      </c>
+      <c r="K605" t="s" s="20">
+        <v>582</v>
       </c>
       <c r="L605" t="s" s="11">
-        <v>6</v>
+        <v>515</v>
       </c>
     </row>
     <row r="606">
-      <c r="A606" s="19"/>
-      <c r="B606" s="19"/>
+      <c r="A606" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B606" s="19" t="s">
+        <v>583</v>
+      </c>
       <c r="C606" s="19"/>
       <c r="D606" s="19"/>
       <c r="E606" s="19"/>
       <c r="F606" s="19"/>
-      <c r="G606" t="s" s="19">
-        <v>4</v>
-      </c>
-      <c r="H606" t="s" s="19">
-        <v>583</v>
-      </c>
-      <c r="I606" t="s" s="45">
-        <v>12</v>
+      <c r="G606" t="s" s="41">
+        <v>0</v>
+      </c>
+      <c r="H606" t="s" s="41">
+        <v>50</v>
+      </c>
+      <c r="I606" t="s" s="41">
+        <v>51</v>
       </c>
       <c r="J606" t="s" s="41">
         <v>0</v>
       </c>
       <c r="K606" t="s" s="41">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="L606" t="s" s="11">
         <v>6</v>
@@ -12193,101 +12187,116 @@
       <c r="D607" s="19"/>
       <c r="E607" s="19"/>
       <c r="F607" s="19"/>
-      <c r="G607" s="19"/>
-      <c r="H607" s="19"/>
-      <c r="I607" s="19"/>
-      <c r="J607" t="s" s="19">
-        <v>4</v>
-      </c>
-      <c r="K607" t="s" s="19">
-        <v>5</v>
+      <c r="G607" t="s" s="19">
+        <v>4</v>
+      </c>
+      <c r="H607" t="s" s="19">
+        <v>584</v>
+      </c>
+      <c r="I607" t="s" s="45">
+        <v>12</v>
+      </c>
+      <c r="J607" t="s" s="41">
+        <v>0</v>
+      </c>
+      <c r="K607" t="s" s="41">
+        <v>52</v>
       </c>
       <c r="L607" t="s" s="11">
         <v>6</v>
       </c>
     </row>
     <row r="608">
-      <c r="B608" s="1" t="s">
+      <c r="A608" s="19"/>
+      <c r="B608" s="19"/>
+      <c r="C608" s="19"/>
+      <c r="D608" s="19"/>
+      <c r="E608" s="19"/>
+      <c r="F608" s="19"/>
+      <c r="G608" s="19"/>
+      <c r="H608" s="19"/>
+      <c r="I608" s="19"/>
+      <c r="J608" t="s" s="19">
+        <v>4</v>
+      </c>
+      <c r="K608" t="s" s="19">
+        <v>5</v>
+      </c>
+      <c r="L608" t="s" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="B609" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C608" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="D608" s="1"/>
-      <c r="E608" s="1"/>
-      <c r="F608" s="1"/>
-    </row>
-    <row r="609">
-      <c r="B609" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C609" s="41" t="s">
+      <c r="C609" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="D609" s="41"/>
-      <c r="E609" s="41"/>
-      <c r="F609" s="41"/>
-      <c r="J609" t="s" s="41">
-        <v>0</v>
-      </c>
-      <c r="K609" t="s" s="41">
-        <v>52</v>
-      </c>
-      <c r="L609" t="s" s="11">
-        <v>6</v>
-      </c>
+      <c r="D609" s="1"/>
+      <c r="E609" s="1"/>
+      <c r="F609" s="1"/>
     </row>
     <row r="610">
       <c r="B610" s="41" t="s">
         <v>0</v>
       </c>
       <c r="C610" s="41" t="s">
-        <v>434</v>
+        <v>586</v>
       </c>
       <c r="D610" s="41"/>
       <c r="E610" s="41"/>
       <c r="F610" s="41"/>
-      <c r="G610" t="s" s="43">
+      <c r="J610" t="s" s="41">
+        <v>0</v>
+      </c>
+      <c r="K610" t="s" s="41">
+        <v>52</v>
+      </c>
+      <c r="L610" t="s" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="B611" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C611" s="41" t="s">
+        <v>434</v>
+      </c>
+      <c r="D611" s="41"/>
+      <c r="E611" s="41"/>
+      <c r="F611" s="41"/>
+      <c r="G611" t="s" s="43">
         <v>68</v>
       </c>
-      <c r="H610" t="s" s="43">
+      <c r="H611" t="s" s="43">
         <v>112</v>
       </c>
-      <c r="I610" t="s" s="41">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="611">
-      <c r="A611" s="27" t="s">
+      <c r="I611" t="s" s="41">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="27" t="s">
         <v>485</v>
       </c>
-      <c r="B611" s="27" t="s">
-        <v>587</v>
-      </c>
-      <c r="C611" s="27"/>
-      <c r="D611" s="27"/>
-      <c r="E611" s="27"/>
-      <c r="F611" s="27"/>
-    </row>
-    <row r="612">
-      <c r="A612" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B612" s="19" t="s">
+      <c r="B612" s="27" t="s">
         <v>588</v>
       </c>
-      <c r="C612" s="19"/>
-      <c r="D612" s="19"/>
-      <c r="E612" s="19"/>
-      <c r="F612" s="19"/>
+      <c r="C612" s="27"/>
+      <c r="D612" s="27"/>
+      <c r="E612" s="27"/>
+      <c r="F612" s="27"/>
     </row>
     <row r="613">
+      <c r="A613" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="B613" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C613" s="19" t="s">
         <v>589</v>
       </c>
+      <c r="C613" s="19"/>
       <c r="D613" s="19"/>
       <c r="E613" s="19"/>
       <c r="F613" s="19"/>
@@ -12424,8 +12433,19 @@
       <c r="E625" s="19"/>
       <c r="F625" s="19"/>
     </row>
+    <row r="626">
+      <c r="B626" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C626" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="D626" s="19"/>
+      <c r="E626" s="19"/>
+      <c r="F626" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="587">
+  <mergeCells count="588">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="C3:F3"/>
@@ -12989,18 +13009,18 @@
     <mergeCell ref="B599:F599"/>
     <mergeCell ref="B600:F600"/>
     <mergeCell ref="A601:F601"/>
-    <mergeCell ref="C602:F602"/>
-    <mergeCell ref="D603:F603"/>
-    <mergeCell ref="C604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="A606:F606"/>
-    <mergeCell ref="A607:I607"/>
-    <mergeCell ref="C608:F608"/>
+    <mergeCell ref="A602:F602"/>
+    <mergeCell ref="C603:F603"/>
+    <mergeCell ref="D604:F604"/>
+    <mergeCell ref="C605:F605"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="A607:F607"/>
+    <mergeCell ref="A608:I608"/>
     <mergeCell ref="C609:F609"/>
     <mergeCell ref="C610:F610"/>
-    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="C611:F611"/>
     <mergeCell ref="B612:F612"/>
-    <mergeCell ref="C613:F613"/>
+    <mergeCell ref="B613:F613"/>
     <mergeCell ref="C614:F614"/>
     <mergeCell ref="C615:F615"/>
     <mergeCell ref="C616:F616"/>
@@ -13013,6 +13033,7 @@
     <mergeCell ref="C623:F623"/>
     <mergeCell ref="C624:F624"/>
     <mergeCell ref="C625:F625"/>
+    <mergeCell ref="C626:F626"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>